<commit_message>
add group/house to website db
</commit_message>
<xml_diff>
--- a/static/excel_sheets/emails.xlsx
+++ b/static/excel_sheets/emails.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benson\Desktop\python projects\gym slot website\static\excel_sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{000AB7AE-D533-4F0D-B002-98ADB5F7A1FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2B703B6-7586-4860-A8E7-1603948AA093}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" xr2:uid="{AB7D5831-8539-4038-A51B-7A0EBE40F72F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>email</t>
   </si>
@@ -47,7 +47,10 @@
     <t>house</t>
   </si>
   <si>
-    <t>year_group</t>
+    <t>group</t>
+  </si>
+  <si>
+    <t>test@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -120,11 +123,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4B809F55-8C75-4399-A116-9FFE08922BC6}" name="Table1" displayName="Table1" ref="A1:C2" totalsRowShown="0" dataCellStyle="Hyperlink">
-  <autoFilter ref="A1:C2" xr:uid="{4B809F55-8C75-4399-A116-9FFE08922BC6}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4B809F55-8C75-4399-A116-9FFE08922BC6}" name="Table1" displayName="Table1" ref="A1:C3" totalsRowShown="0" dataCellStyle="Hyperlink">
+  <autoFilter ref="A1:C3" xr:uid="{4B809F55-8C75-4399-A116-9FFE08922BC6}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{E3B05914-5AE5-445A-AAFD-D012335F9AFA}" name="email" dataCellStyle="Hyperlink"/>
-    <tableColumn id="3" xr3:uid="{81468965-C3E4-4BBC-A5DB-B2C8D529097C}" name="year_group" dataCellStyle="Hyperlink"/>
+    <tableColumn id="3" xr3:uid="{81468965-C3E4-4BBC-A5DB-B2C8D529097C}" name="group" dataCellStyle="Hyperlink"/>
     <tableColumn id="4" xr3:uid="{74AC6803-911D-49CC-AF6E-733725653D38}" name="house" dataCellStyle="Hyperlink"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -428,10 +431,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6A8A12E-95C0-4A7B-92E4-5E1CD7C60755}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="128" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -461,15 +464,27 @@
         <v>1</v>
       </c>
     </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1">
+        <v>11</v>
+      </c>
+      <c r="C3" s="1">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{447A608E-BC83-4229-9611-F189B836CCD0}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{54AACFC6-A58E-41C7-B322-82E665CBEDA0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>